<commit_message>
First attempt at refactoring
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
@@ -21,16 +21,8 @@
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
   <x:pivotCaches>
-    <x:pivotCache cacheId="0" r:id="rId16"/>
-    <x:pivotCache cacheId="1" r:id="rId19"/>
-    <x:pivotCache cacheId="2" r:id="rId22"/>
-    <x:pivotCache cacheId="3" r:id="rId25"/>
-    <x:pivotCache cacheId="4" r:id="rId28"/>
-    <x:pivotCache cacheId="5" r:id="rId31"/>
-    <x:pivotCache cacheId="6" r:id="rId34"/>
-    <x:pivotCache cacheId="7" r:id="rId37"/>
-    <x:pivotCache cacheId="8" r:id="rId40"/>
-    <x:pivotCache cacheId="9" r:id="rId43"/>
+    <x:pivotCache cacheId="0" r:id="rId15"/>
+    <x:pivotCache cacheId="1" r:id="rId16"/>
   </x:pivotCaches>
 </x:workbook>
 </file>
@@ -232,7 +224,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtInteger" cacheId="9" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtInteger" cacheId="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -405,7 +397,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="1" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="0" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -484,7 +476,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="2" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="0" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -564,7 +556,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtNoColumnLabels" cacheId="3" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1" rowHeaderCaption="Pastry name">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtNoColumnLabels" cacheId="0" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1" rowHeaderCaption="Pastry name">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -649,7 +641,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtCollapsedFields" cacheId="4" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtCollapsedFields" cacheId="0" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisRow" allDrilled="1" showAll="0" defaultSubtotal="0">
@@ -734,7 +726,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtFieldAsValueAndLabel" cacheId="5" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtFieldAsValueAndLabel" cacheId="0" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisRow" dataField="1" showAll="0" defaultSubtotal="0">
@@ -812,7 +804,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtHidesubTotals" cacheId="6" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1" colHeaderCaption="Measures">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtHidesubTotals" cacheId="0" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1" colHeaderCaption="Measures">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisCol" showAll="0" defaultSubtotal="0">
@@ -889,7 +881,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtFilter" cacheId="7" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtFilter" cacheId="0" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
   <x:location ref="A5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisPage" multipleItemSelectionAllowed="1" showAll="0" defaultSubtotal="0">
@@ -990,7 +982,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtSort" cacheId="8" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1" rowHeaderCaption="Pastry name">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtSort" cacheId="0" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1" rowHeaderCaption="Pastry name">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisRow" showAll="0" sortType="ascending" defaultSubtotal="0">
@@ -1728,7 +1720,7 @@
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
   <x:tableParts count="1">
-    <x:tablePart r:id="rId15"/>
+    <x:tablePart r:id="rId17"/>
   </x:tableParts>
 </x:worksheet>
 </file>
@@ -1942,7 +1934,7 @@
   </x:cacheSource>
   <x:cacheFields>
     <x:cacheField name="Name">
-      <x:sharedItems count="5">
+      <x:sharedItems>
         <x:s v="Croissant"/>
         <x:s v="Doughnut"/>
         <x:s v="Bearclaw"/>
@@ -1951,339 +1943,13 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="Code">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
+      <x:sharedItems/>
     </x:cacheField>
     <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="14"/>
+      <x:sharedItems/>
     </x:cacheField>
     <x:cacheField name="Quality">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="16"/>
-    </x:cacheField>
-    <x:cacheField name="Month">
-      <x:sharedItems count="3">
-        <x:s v="Apr"/>
-        <x:s v="May"/>
-        <x:s v="Jun"/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
-    </x:cacheField>
-  </x:cacheFields>
-</x:pivotCacheDefinition>
-</file>
-
-<file path=pivotCache/pivotCacheDefinition10.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
-  <x:cacheSource type="worksheet">
-    <x:worksheetSource name="PastrySalesData"/>
-  </x:cacheSource>
-  <x:cacheFields>
-    <x:cacheField name="Name">
-      <x:sharedItems count="5">
-        <x:s v="Croissant"/>
-        <x:s v="Doughnut"/>
-        <x:s v="Bearclaw"/>
-        <x:s v="Danish"/>
-        <x:s v="Scone"/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="Code">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5">
-        <x:n v="101"/>
-        <x:n v="102"/>
-        <x:n v="103"/>
-        <x:n v="104"/>
-        <x:n v="105"/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="14"/>
-    </x:cacheField>
-    <x:cacheField name="Quality">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="16"/>
-    </x:cacheField>
-    <x:cacheField name="Month">
-      <x:sharedItems count="3">
-        <x:s v="Apr"/>
-        <x:s v="May"/>
-        <x:s v="Jun"/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15">
-        <x:d v="2016-04-21T00:00:00"/>
-        <x:d v="2016-05-03T00:00:00"/>
-        <x:d v="2016-06-24T00:00:00"/>
-        <x:d v="2017-04-23T00:00:00"/>
-        <x:d v="2016-05-24T00:00:00"/>
-        <x:d v="2016-06-02T00:00:00"/>
-        <x:d v="2016-04-27T00:00:00"/>
-        <x:d v="2016-05-20T00:00:00"/>
-        <x:d v="2017-06-05T00:00:00"/>
-        <x:d v="2017-04-24T00:00:00"/>
-        <x:d v="2017-05-08T00:00:00"/>
-        <x:d v="2016-06-21T00:00:00"/>
-        <x:d v="2017-04-22T00:00:00"/>
-        <x:d v="2017-05-03T00:00:00"/>
-        <x:d v="2017-06-14T00:00:00"/>
-      </x:sharedItems>
-    </x:cacheField>
-  </x:cacheFields>
-</x:pivotCacheDefinition>
-</file>
-
-<file path=pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
-  <x:cacheSource type="worksheet">
-    <x:worksheetSource ref="A1:F17" sheet="PastrySalesData"/>
-  </x:cacheSource>
-  <x:cacheFields>
-    <x:cacheField name="Name">
-      <x:sharedItems count="5">
-        <x:s v="Croissant"/>
-        <x:s v="Doughnut"/>
-        <x:s v="Bearclaw"/>
-        <x:s v="Danish"/>
-        <x:s v="Scone"/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="Code">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
-    </x:cacheField>
-    <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="14"/>
-    </x:cacheField>
-    <x:cacheField name="Quality">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="16"/>
-    </x:cacheField>
-    <x:cacheField name="Month">
-      <x:sharedItems count="3">
-        <x:s v="Apr"/>
-        <x:s v="May"/>
-        <x:s v="Jun"/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
-    </x:cacheField>
-  </x:cacheFields>
-</x:pivotCacheDefinition>
-</file>
-
-<file path=pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
-  <x:cacheSource type="worksheet">
-    <x:worksheetSource ref="A1:F17" sheet="PastrySalesData"/>
-  </x:cacheSource>
-  <x:cacheFields>
-    <x:cacheField name="Name">
-      <x:sharedItems count="5">
-        <x:s v="Croissant"/>
-        <x:s v="Doughnut"/>
-        <x:s v="Bearclaw"/>
-        <x:s v="Danish"/>
-        <x:s v="Scone"/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="Code">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
-    </x:cacheField>
-    <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="14"/>
-    </x:cacheField>
-    <x:cacheField name="Quality">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="16"/>
-    </x:cacheField>
-    <x:cacheField name="Month">
-      <x:sharedItems count="3">
-        <x:s v="Apr"/>
-        <x:s v="May"/>
-        <x:s v="Jun"/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
-    </x:cacheField>
-  </x:cacheFields>
-</x:pivotCacheDefinition>
-</file>
-
-<file path=pivotCache/pivotCacheDefinition4.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
-  <x:cacheSource type="worksheet">
-    <x:worksheetSource ref="A1:F17" sheet="PastrySalesData"/>
-  </x:cacheSource>
-  <x:cacheFields>
-    <x:cacheField name="Name">
-      <x:sharedItems count="5">
-        <x:s v="Croissant"/>
-        <x:s v="Doughnut"/>
-        <x:s v="Bearclaw"/>
-        <x:s v="Danish"/>
-        <x:s v="Scone"/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="Code">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
-    </x:cacheField>
-    <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="14"/>
-    </x:cacheField>
-    <x:cacheField name="Quality">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="16"/>
-    </x:cacheField>
-    <x:cacheField name="Month">
-      <x:sharedItems count="3">
-        <x:s v="Apr"/>
-        <x:s v="May"/>
-        <x:s v="Jun"/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
-    </x:cacheField>
-  </x:cacheFields>
-</x:pivotCacheDefinition>
-</file>
-
-<file path=pivotCache/pivotCacheDefinition5.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
-  <x:cacheSource type="worksheet">
-    <x:worksheetSource ref="A1:F17" sheet="PastrySalesData"/>
-  </x:cacheSource>
-  <x:cacheFields>
-    <x:cacheField name="Name">
-      <x:sharedItems count="5">
-        <x:s v="Croissant"/>
-        <x:s v="Doughnut"/>
-        <x:s v="Bearclaw"/>
-        <x:s v="Danish"/>
-        <x:s v="Scone"/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="Code">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
-    </x:cacheField>
-    <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="14"/>
-    </x:cacheField>
-    <x:cacheField name="Quality">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="16"/>
-    </x:cacheField>
-    <x:cacheField name="Month">
-      <x:sharedItems count="3">
-        <x:s v="Apr"/>
-        <x:s v="May"/>
-        <x:s v="Jun"/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
-    </x:cacheField>
-  </x:cacheFields>
-</x:pivotCacheDefinition>
-</file>
-
-<file path=pivotCache/pivotCacheDefinition6.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
-  <x:cacheSource type="worksheet">
-    <x:worksheetSource ref="A1:F17" sheet="PastrySalesData"/>
-  </x:cacheSource>
-  <x:cacheFields>
-    <x:cacheField name="Name">
-      <x:sharedItems count="5">
-        <x:s v="Croissant"/>
-        <x:s v="Doughnut"/>
-        <x:s v="Bearclaw"/>
-        <x:s v="Danish"/>
-        <x:s v="Scone"/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="Code">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
-    </x:cacheField>
-    <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="14"/>
-    </x:cacheField>
-    <x:cacheField name="Quality">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="16"/>
-    </x:cacheField>
-    <x:cacheField name="Month">
-      <x:sharedItems count="3">
-        <x:s v="Apr"/>
-        <x:s v="May"/>
-        <x:s v="Jun"/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
-    </x:cacheField>
-  </x:cacheFields>
-</x:pivotCacheDefinition>
-</file>
-
-<file path=pivotCache/pivotCacheDefinition7.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
-  <x:cacheSource type="worksheet">
-    <x:worksheetSource ref="A1:F17" sheet="PastrySalesData"/>
-  </x:cacheSource>
-  <x:cacheFields>
-    <x:cacheField name="Name">
-      <x:sharedItems count="5">
-        <x:s v="Croissant"/>
-        <x:s v="Doughnut"/>
-        <x:s v="Bearclaw"/>
-        <x:s v="Danish"/>
-        <x:s v="Scone"/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="Code">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
-    </x:cacheField>
-    <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="14"/>
-    </x:cacheField>
-    <x:cacheField name="Quality">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="16"/>
-    </x:cacheField>
-    <x:cacheField name="Month">
-      <x:sharedItems count="3">
-        <x:s v="Apr"/>
-        <x:s v="May"/>
-        <x:s v="Jun"/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
-    </x:cacheField>
-  </x:cacheFields>
-</x:pivotCacheDefinition>
-</file>
-
-<file path=pivotCache/pivotCacheDefinition8.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
-  <x:cacheSource type="worksheet">
-    <x:worksheetSource ref="A1:F17" sheet="PastrySalesData"/>
-  </x:cacheSource>
-  <x:cacheFields>
-    <x:cacheField name="Name">
-      <x:sharedItems count="5">
-        <x:s v="Croissant"/>
-        <x:s v="Doughnut"/>
-        <x:s v="Bearclaw"/>
-        <x:s v="Danish"/>
-        <x:s v="Scone"/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="Code">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
-    </x:cacheField>
-    <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="14"/>
-    </x:cacheField>
-    <x:cacheField name="Quality">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="16">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99">
         <x:n v="60.2"/>
         <x:n v="50.42"/>
         <x:n v="22.12"/>
@@ -2303,43 +1969,43 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="Month">
-      <x:sharedItems count="3">
+      <x:sharedItems>
         <x:s v="Apr"/>
         <x:s v="May"/>
         <x:s v="Jun"/>
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15">
-        <x:d v="2016-04-21T00:00:00"/>
-        <x:d v="2016-05-03T00:00:00"/>
-        <x:d v="2016-06-24T00:00:00"/>
-        <x:d v="2017-04-23T00:00:00"/>
-        <x:d v="2016-05-24T00:00:00"/>
-        <x:d v="2016-06-02T00:00:00"/>
-        <x:d v="2016-04-27T00:00:00"/>
-        <x:d v="2016-05-20T00:00:00"/>
-        <x:d v="2017-06-05T00:00:00"/>
-        <x:d v="2017-04-24T00:00:00"/>
-        <x:d v="2017-05-08T00:00:00"/>
-        <x:d v="2016-06-21T00:00:00"/>
-        <x:d v="2017-04-22T00:00:00"/>
-        <x:d v="2017-05-03T00:00:00"/>
-        <x:d v="2017-06-14T00:00:00"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00Z" maxDate="2017-06-14T00:00:00Z">
+        <x:d v="2016-04-21T00:00:00Z"/>
+        <x:d v="2016-05-03T00:00:00Z"/>
+        <x:d v="2016-06-24T00:00:00Z"/>
+        <x:d v="2017-04-23T00:00:00Z"/>
+        <x:d v="2016-05-24T00:00:00Z"/>
+        <x:d v="2016-06-02T00:00:00Z"/>
+        <x:d v="2016-04-27T00:00:00Z"/>
+        <x:d v="2016-05-20T00:00:00Z"/>
+        <x:d v="2017-06-05T00:00:00Z"/>
+        <x:d v="2017-04-24T00:00:00Z"/>
+        <x:d v="2017-05-08T00:00:00Z"/>
+        <x:d v="2016-06-21T00:00:00Z"/>
+        <x:d v="2017-04-22T00:00:00Z"/>
+        <x:d v="2017-05-03T00:00:00Z"/>
+        <x:d v="2017-06-14T00:00:00Z"/>
       </x:sharedItems>
     </x:cacheField>
   </x:cacheFields>
 </x:pivotCacheDefinition>
 </file>
 
-<file path=pivotCache/pivotCacheDefinition9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
   <x:cacheSource type="worksheet">
-    <x:worksheetSource ref="A1:F17" sheet="PastrySalesData"/>
+    <x:worksheetSource name="PastrySalesData"/>
   </x:cacheSource>
   <x:cacheFields>
     <x:cacheField name="Name">
-      <x:sharedItems count="5">
+      <x:sharedItems>
         <x:s v="Croissant"/>
         <x:s v="Doughnut"/>
         <x:s v="Bearclaw"/>
@@ -2348,23 +2014,45 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="Code">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="101" maxValue="105">
+        <x:n v="101"/>
+        <x:n v="102"/>
+        <x:n v="103"/>
+        <x:n v="104"/>
+        <x:n v="105"/>
+      </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="14"/>
+      <x:sharedItems/>
     </x:cacheField>
     <x:cacheField name="Quality">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="16"/>
+      <x:sharedItems/>
     </x:cacheField>
     <x:cacheField name="Month">
-      <x:sharedItems count="3">
+      <x:sharedItems>
         <x:s v="Apr"/>
         <x:s v="May"/>
         <x:s v="Jun"/>
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00Z" maxDate="2017-06-14T00:00:00Z">
+        <x:d v="2016-04-21T00:00:00Z"/>
+        <x:d v="2016-05-03T00:00:00Z"/>
+        <x:d v="2016-06-24T00:00:00Z"/>
+        <x:d v="2017-04-23T00:00:00Z"/>
+        <x:d v="2016-05-24T00:00:00Z"/>
+        <x:d v="2016-06-02T00:00:00Z"/>
+        <x:d v="2016-04-27T00:00:00Z"/>
+        <x:d v="2016-05-20T00:00:00Z"/>
+        <x:d v="2017-06-05T00:00:00Z"/>
+        <x:d v="2017-04-24T00:00:00Z"/>
+        <x:d v="2017-05-08T00:00:00Z"/>
+        <x:d v="2016-06-21T00:00:00Z"/>
+        <x:d v="2017-04-22T00:00:00Z"/>
+        <x:d v="2017-05-03T00:00:00Z"/>
+        <x:d v="2017-06-14T00:00:00Z"/>
+      </x:sharedItems>
     </x:cacheField>
   </x:cacheFields>
 </x:pivotCacheDefinition>
@@ -2374,38 +2062,6 @@
 <x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
-<file path=pivotCache/pivotCacheRecords10.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=pivotCache/pivotCacheRecords3.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=pivotCache/pivotCacheRecords4.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=pivotCache/pivotCacheRecords5.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=pivotCache/pivotCacheRecords6.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=pivotCache/pivotCacheRecords7.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=pivotCache/pivotCacheRecords8.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=pivotCache/pivotCacheRecords9.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
</xml_diff>